<commit_message>
Entrega2 Planilha teste Local do resultado
</commit_message>
<xml_diff>
--- a/grupo2/AulaElias05.04ValidadoGrupo1.xlsx
+++ b/grupo2/AulaElias05.04ValidadoGrupo1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Entrada (Salário; Qtde de dependentes)</t>
   </si>
@@ -49,7 +49,10 @@
     <t>(1260,00;120,00;120,00;00,00)</t>
   </si>
   <si>
-    <t>Falha SL:1380,00 </t>
+    <t> </t>
+  </si>
+  <si>
+    <t>Falha SL:1380,00</t>
   </si>
   <si>
     <t>(1.800,00;1)</t>
@@ -76,8 +79,7 @@
     <t>(420,00;40,00;72,00;00,00)</t>
   </si>
   <si>
-    <t>Falha SL: O valor do salario não pode ser menor que o salario minimo!!!!!Digite o valor do salario novamente:
- </t>
+    <t>Falha SL: O valor do salario não pode ser menor que o salario minimo!!!!!Digite o valor do salario novamente:</t>
   </si>
   <si>
     <t>(900,00;1)</t>
@@ -95,9 +97,6 @@
     <t>(588,00;56,00;56,00;00,00)</t>
   </si>
   <si>
-    <t>Falha SL: O valor do salario não pode ser menor que o salario minimo!!!!!Digite o valor do salario novamente:</t>
-  </si>
-  <si>
     <t>(800,00;1)</t>
   </si>
   <si>
@@ -110,7 +109,7 @@
     <t>(924,00;88,00;88,00;00,00)</t>
   </si>
   <si>
-    <t>Falha= 963,00 IR= 48,17</t>
+    <t>Falha= SL: 1112,00</t>
   </si>
 </sst>
 </file>
@@ -243,12 +242,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -274,17 +273,17 @@
   </sheetPr>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.3877551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.5102040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.5459183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.7040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="14.3826530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.9795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.1479591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.2295918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.3877551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="14.2295918367347"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -309,10 +308,10 @@
       <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5"/>
       <c r="E2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -325,71 +324,73 @@
       <c r="C3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="5"/>
+      <c r="D3" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="E3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="E4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="5"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="E6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="5"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="5"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
@@ -398,10 +399,10 @@
       <c r="B9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="5"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
@@ -410,10 +411,10 @@
       <c r="B10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="8"/>
+      <c r="D10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>